<commit_message>
Similarity Checking Done. UI changes. Fixed bugs.
</commit_message>
<xml_diff>
--- a/backend/processing/templates/download/question-bank-tpl-clean.xlsx
+++ b/backend/processing/templates/download/question-bank-tpl-clean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Assumption University\Senior Project 1\SeniorProject1\backend\processing\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AU\3rd-Year_2nd-Sem\CSX3010-SP1\SeniorProject1\backend\processing\templates\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BE7131-5D25-424C-988B-5146AFBD075D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3130BA7C-93B4-4839-8632-7554E27CFD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
+    <workbookView xWindow="3084" yWindow="2688" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Semester</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Exam Type</t>
+  </si>
+  <si>
+    <t>PLEASE EDIT WITHOUT CHANGING FORMULA.</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +144,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,18 +166,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="18" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,246 +533,263 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16" width="8.88671875" style="2"/>
+    <col min="17" max="17" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="2">
         <f ca="1">IF(Q3&lt;6,Q2-1,Q2)</f>
         <v>2025</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="3">
+      <c r="Q1" s="6">
         <f ca="1">TODAY()</f>
-        <v>45895</v>
+        <v>45914</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <f ca="1">VLOOKUP(Q3,P5:R17,3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="2">
         <f ca="1">YEAR(Q1)</f>
         <v>2025</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" s="2" t="str">
         <f ca="1">VLOOKUP(Q3,P6:R17,2,FALSE)</f>
-        <v>MIDTERM</v>
-      </c>
-      <c r="P3" t="s">
+        <v>FINAL</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="2">
         <f ca="1">MONTH(Q1)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="P5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="P6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P7" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="P8" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="P5" t="s">
+      <c r="B9" s="3"/>
+      <c r="P9" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" s="2">
         <v>3</v>
       </c>
-      <c r="Q5" t="s">
-        <v>4</v>
-      </c>
-      <c r="R5" t="s">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="P10" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="P6">
+      <c r="Q10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P11" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R11" s="2">
         <v>1</v>
       </c>
-      <c r="Q6" t="s">
-        <v>7</v>
-      </c>
-      <c r="R6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="P7">
-        <v>2</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>6</v>
-      </c>
-      <c r="R7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="P8">
-        <v>3</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>6</v>
-      </c>
-      <c r="R8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="P9">
-        <v>4</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="P10">
-        <v>5</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>6</v>
-      </c>
-      <c r="R10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="P11">
-        <v>6</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>7</v>
-      </c>
-      <c r="R11">
-        <v>1</v>
-      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <f>DATE(2025,6,10)</f>
         <v>45818</v>
       </c>
-      <c r="P12">
+      <c r="E12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="P12" s="2">
         <v>7</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <f>TIME(9,0,0)</f>
         <v>0.375</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <f>TIME(12,0,0)</f>
         <v>0.5</v>
       </c>
-      <c r="P13">
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="P13" s="2">
         <v>8</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="P14">
+      <c r="P14" s="2">
         <v>9</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="P15">
+      <c r="P15" s="2">
         <v>10</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="Q15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="P16">
+      <c r="P16" s="2">
         <v>11</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="16:18" x14ac:dyDescent="0.3">
-      <c r="P17">
+      <c r="P17" s="2">
         <v>12</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="2">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E12:I13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -755,41 +799,42 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.44140625" customWidth="1"/>
-    <col min="2" max="6" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="66.44140625" style="1" customWidth="1"/>
+    <col min="2" max="6" width="15.77734375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -801,28 +846,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589423D0-50CB-4F3F-82F4-CB353E932D78}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C41"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -832,129 +881,138 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFE4AC3-D33B-41F7-AFE1-650B291E6FA6}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.44140625" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="gSUsP0iwppKqmD7FA3P+gzSD+R2vya95kS2axiasengYkTZzXhqFK/49tSstrno7Nx91FjjkuZAey3cf7NxIng==" saltValue="ovpBf8V71Srjh/GO4U6cAQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15F7917-4FC8-4FF7-B762-EA8CF8ABB661}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5"/>
-      <c r="B5" s="1"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+      <c r="E1" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="10"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+    </row>
+    <row r="7" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+    </row>
+    <row r="11" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+    </row>
+    <row r="12" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+    </row>
+    <row r="15" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+    </row>
+    <row r="16" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
     </row>
     <row r="17" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+      <c r="A17" s="10"/>
     </row>
     <row r="18" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+      <c r="A18" s="10"/>
     </row>
     <row r="19" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+      <c r="A19" s="10"/>
     </row>
     <row r="20" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+      <c r="A20" s="10"/>
     </row>
     <row r="21" spans="1:1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+      <c r="A21" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>